<commit_message>
Adição plano projeto cronograma
Adição do plano do projeto e do cronograma do projeto
</commit_message>
<xml_diff>
--- a/PLA-Planilha de Avaliação .xlsx
+++ b/PLA-Planilha de Avaliação .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções para preenchimento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="104">
   <si>
     <t>INSTRUÇÕES</t>
   </si>
@@ -540,14 +540,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFF99"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1066,9 +1066,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1106,48 +1103,48 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1172,6 +1169,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1777,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="41"/>
-      <c r="D5" s="81"/>
+      <c r="D5" s="80"/>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
@@ -1922,11 +1922,11 @@
       <c r="B6" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="82" t="s">
+      <c r="C6" s="79"/>
+      <c r="D6" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="79"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -1948,8 +1948,8 @@
       <c r="B7" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="83" t="s">
+      <c r="C7" s="79"/>
+      <c r="D7" s="82" t="s">
         <v>98</v>
       </c>
       <c r="E7" s="25"/>
@@ -2055,7 +2055,7 @@
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="41"/>
-      <c r="D12" s="81"/>
+      <c r="D12" s="80"/>
       <c r="E12" s="41"/>
       <c r="F12" s="41"/>
       <c r="G12" s="41"/>
@@ -2072,17 +2072,17 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="83" t="s">
         <v>99</v>
       </c>
       <c r="B13" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="80"/>
-      <c r="D13" s="82" t="s">
+      <c r="C13" s="79"/>
+      <c r="D13" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="79"/>
+      <c r="E13" s="78"/>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -2098,14 +2098,14 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="83" t="s">
         <v>101</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="82" t="s">
+      <c r="C14" s="79"/>
+      <c r="D14" s="81" t="s">
         <v>98</v>
       </c>
       <c r="E14" s="25"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
-      <c r="D19" s="81"/>
+      <c r="D19" s="80"/>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
       <c r="G19" s="41"/>
@@ -2234,11 +2234,11 @@
       <c r="B20" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="80"/>
-      <c r="D20" s="82" t="s">
+      <c r="C20" s="79"/>
+      <c r="D20" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="79"/>
+      <c r="E20" s="78"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
@@ -2256,8 +2256,8 @@
     <row r="21" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23"/>
       <c r="B21" s="24"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="85"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="84"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
@@ -2385,10 +2385,10 @@
         <v>100</v>
       </c>
       <c r="C27" s="25"/>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="79"/>
+      <c r="E27" s="78"/>
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
@@ -2535,11 +2535,10 @@
         <v>60</v>
       </c>
       <c r="C34" s="25"/>
-      <c r="D34" s="26" t="str">
-        <f>HYPERLINK("https://drive.google.com/open?id=1TxlGDIUf96mTtncwmoUifoawKayBmM-XL1cQxXnAO_I&amp;authuser=1","x")</f>
-        <v>x</v>
-      </c>
-      <c r="E34" s="47"/>
+      <c r="D34" s="85" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="86"/>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
@@ -2635,16 +2634,16 @@
       <c r="R38" s="1"/>
     </row>
     <row r="39" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="48"/>
-      <c r="B39" s="49" t="s">
+      <c r="A39" s="47"/>
+      <c r="B39" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="52"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="51"/>
       <c r="I39" s="7"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -2657,14 +2656,14 @@
       <c r="R39" s="1"/>
     </row>
     <row r="40" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="53"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
       <c r="I40" s="7"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -2677,16 +2676,16 @@
       <c r="R40" s="1"/>
     </row>
     <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="58"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="57"/>
       <c r="I41" s="7"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -2699,16 +2698,16 @@
       <c r="R41" s="1"/>
     </row>
     <row r="42" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="59" t="s">
+      <c r="A42" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="62"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="61"/>
       <c r="I42" s="7"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -2721,16 +2720,16 @@
       <c r="R42" s="1"/>
     </row>
     <row r="43" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="63" t="s">
+      <c r="A43" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="64"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="66"/>
-      <c r="H43" s="66"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
       <c r="I43" s="7"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -2743,16 +2742,16 @@
       <c r="R43" s="1"/>
     </row>
     <row r="44" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="70"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
       <c r="I44" s="7"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -2887,16 +2886,16 @@
       <c r="R50" s="1"/>
     </row>
     <row r="51" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="71" t="s">
+      <c r="A51" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="72"/>
-      <c r="C51" s="73"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="70"/>
-      <c r="H51" s="70"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="72"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
       <c r="I51" s="7"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -2909,16 +2908,16 @@
       <c r="R51" s="1"/>
     </row>
     <row r="52" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="74" t="s">
+      <c r="A52" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="76"/>
-      <c r="G52" s="70"/>
-      <c r="H52" s="70"/>
+      <c r="B52" s="74"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="69"/>
       <c r="I52" s="7"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -3053,16 +3052,16 @@
       <c r="R58" s="1"/>
     </row>
     <row r="59" spans="1:18" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="74" t="s">
+      <c r="A59" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="77"/>
-      <c r="C59" s="78"/>
-      <c r="D59" s="78"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="78"/>
-      <c r="G59" s="70"/>
-      <c r="H59" s="70"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="77"/>
+      <c r="D59" s="77"/>
+      <c r="E59" s="77"/>
+      <c r="F59" s="77"/>
+      <c r="G59" s="69"/>
+      <c r="H59" s="69"/>
       <c r="I59" s="7"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
@@ -3197,16 +3196,16 @@
       <c r="R65" s="1"/>
     </row>
     <row r="66" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="74" t="s">
+      <c r="A66" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="78"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
-      <c r="F66" s="78"/>
-      <c r="G66" s="70"/>
-      <c r="H66" s="70"/>
+      <c r="B66" s="77"/>
+      <c r="C66" s="77"/>
+      <c r="D66" s="77"/>
+      <c r="E66" s="77"/>
+      <c r="F66" s="77"/>
+      <c r="G66" s="69"/>
+      <c r="H66" s="69"/>
       <c r="I66" s="7"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -3341,16 +3340,16 @@
       <c r="R72" s="1"/>
     </row>
     <row r="73" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="74" t="s">
+      <c r="A73" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="78"/>
-      <c r="C73" s="78"/>
-      <c r="D73" s="78"/>
-      <c r="E73" s="78"/>
-      <c r="F73" s="78"/>
-      <c r="G73" s="70"/>
-      <c r="H73" s="70"/>
+      <c r="B73" s="77"/>
+      <c r="C73" s="77"/>
+      <c r="D73" s="77"/>
+      <c r="E73" s="77"/>
+      <c r="F73" s="77"/>
+      <c r="G73" s="69"/>
+      <c r="H73" s="69"/>
       <c r="I73" s="7"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -3485,16 +3484,16 @@
       <c r="R79" s="1"/>
     </row>
     <row r="80" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="74" t="s">
+      <c r="A80" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="78"/>
-      <c r="C80" s="78"/>
-      <c r="D80" s="78"/>
-      <c r="E80" s="78"/>
-      <c r="F80" s="78"/>
-      <c r="G80" s="70"/>
-      <c r="H80" s="70"/>
+      <c r="B80" s="77"/>
+      <c r="C80" s="77"/>
+      <c r="D80" s="77"/>
+      <c r="E80" s="77"/>
+      <c r="F80" s="77"/>
+      <c r="G80" s="69"/>
+      <c r="H80" s="69"/>
       <c r="I80" s="7"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
@@ -3629,16 +3628,16 @@
       <c r="R86" s="1"/>
     </row>
     <row r="87" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="74" t="s">
+      <c r="A87" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="78"/>
-      <c r="C87" s="78"/>
-      <c r="D87" s="78"/>
-      <c r="E87" s="78"/>
-      <c r="F87" s="78"/>
-      <c r="G87" s="70"/>
-      <c r="H87" s="70"/>
+      <c r="B87" s="77"/>
+      <c r="C87" s="77"/>
+      <c r="D87" s="77"/>
+      <c r="E87" s="77"/>
+      <c r="F87" s="77"/>
+      <c r="G87" s="69"/>
+      <c r="H87" s="69"/>
       <c r="I87" s="7"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
@@ -3773,16 +3772,16 @@
       <c r="R93" s="1"/>
     </row>
     <row r="94" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="74" t="s">
+      <c r="A94" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="B94" s="78"/>
-      <c r="C94" s="78"/>
-      <c r="D94" s="78"/>
-      <c r="E94" s="78"/>
-      <c r="F94" s="78"/>
-      <c r="G94" s="70"/>
-      <c r="H94" s="70"/>
+      <c r="B94" s="77"/>
+      <c r="C94" s="77"/>
+      <c r="D94" s="77"/>
+      <c r="E94" s="77"/>
+      <c r="F94" s="77"/>
+      <c r="G94" s="69"/>
+      <c r="H94" s="69"/>
       <c r="I94" s="7"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
@@ -3917,16 +3916,16 @@
       <c r="R100" s="1"/>
     </row>
     <row r="101" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="74" t="s">
+      <c r="A101" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="B101" s="78"/>
-      <c r="C101" s="78"/>
-      <c r="D101" s="78"/>
-      <c r="E101" s="78"/>
-      <c r="F101" s="78"/>
-      <c r="G101" s="70"/>
-      <c r="H101" s="70"/>
+      <c r="B101" s="77"/>
+      <c r="C101" s="77"/>
+      <c r="D101" s="77"/>
+      <c r="E101" s="77"/>
+      <c r="F101" s="77"/>
+      <c r="G101" s="69"/>
+      <c r="H101" s="69"/>
       <c r="I101" s="7"/>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
@@ -4061,16 +4060,16 @@
       <c r="R107" s="1"/>
     </row>
     <row r="108" spans="1:18" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="74" t="s">
+      <c r="A108" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="B108" s="78"/>
-      <c r="C108" s="78"/>
-      <c r="D108" s="78"/>
-      <c r="E108" s="78"/>
-      <c r="F108" s="78"/>
-      <c r="G108" s="70"/>
-      <c r="H108" s="70"/>
+      <c r="B108" s="77"/>
+      <c r="C108" s="77"/>
+      <c r="D108" s="77"/>
+      <c r="E108" s="77"/>
+      <c r="F108" s="77"/>
+      <c r="G108" s="69"/>
+      <c r="H108" s="69"/>
       <c r="I108" s="7"/>
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
@@ -4205,16 +4204,16 @@
       <c r="R114" s="1"/>
     </row>
     <row r="115" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="74" t="s">
+      <c r="A115" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="B115" s="78"/>
-      <c r="C115" s="78"/>
-      <c r="D115" s="78"/>
-      <c r="E115" s="78"/>
-      <c r="F115" s="78"/>
-      <c r="G115" s="70"/>
-      <c r="H115" s="70"/>
+      <c r="B115" s="77"/>
+      <c r="C115" s="77"/>
+      <c r="D115" s="77"/>
+      <c r="E115" s="77"/>
+      <c r="F115" s="77"/>
+      <c r="G115" s="69"/>
+      <c r="H115" s="69"/>
       <c r="I115" s="7"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
@@ -4349,16 +4348,16 @@
       <c r="R121" s="1"/>
     </row>
     <row r="122" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="74" t="s">
+      <c r="A122" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B122" s="78"/>
-      <c r="C122" s="78"/>
-      <c r="D122" s="78"/>
-      <c r="E122" s="78"/>
-      <c r="F122" s="78"/>
-      <c r="G122" s="70"/>
-      <c r="H122" s="70"/>
+      <c r="B122" s="77"/>
+      <c r="C122" s="77"/>
+      <c r="D122" s="77"/>
+      <c r="E122" s="77"/>
+      <c r="F122" s="77"/>
+      <c r="G122" s="69"/>
+      <c r="H122" s="69"/>
       <c r="I122" s="7"/>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
@@ -4493,16 +4492,16 @@
       <c r="R128" s="1"/>
     </row>
     <row r="129" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="74" t="s">
+      <c r="A129" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="B129" s="78"/>
-      <c r="C129" s="78"/>
-      <c r="D129" s="78"/>
-      <c r="E129" s="78"/>
-      <c r="F129" s="78"/>
-      <c r="G129" s="70"/>
-      <c r="H129" s="70"/>
+      <c r="B129" s="77"/>
+      <c r="C129" s="77"/>
+      <c r="D129" s="77"/>
+      <c r="E129" s="77"/>
+      <c r="F129" s="77"/>
+      <c r="G129" s="69"/>
+      <c r="H129" s="69"/>
       <c r="I129" s="7"/>
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
@@ -4637,16 +4636,16 @@
       <c r="R135" s="1"/>
     </row>
     <row r="136" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="74" t="s">
+      <c r="A136" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="B136" s="78"/>
-      <c r="C136" s="78"/>
-      <c r="D136" s="78"/>
-      <c r="E136" s="78"/>
-      <c r="F136" s="78"/>
-      <c r="G136" s="70"/>
-      <c r="H136" s="70"/>
+      <c r="B136" s="77"/>
+      <c r="C136" s="77"/>
+      <c r="D136" s="77"/>
+      <c r="E136" s="77"/>
+      <c r="F136" s="77"/>
+      <c r="G136" s="69"/>
+      <c r="H136" s="69"/>
       <c r="I136" s="7"/>
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
@@ -4782,13 +4781,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D34" r:id="rId1" display="https://drive.google.com/open?id=1TxlGDIUf96mTtncwmoUifoawKayBmM-XL1cQxXnAO_I&amp;authuser=1"/>
-    <hyperlink ref="D6" r:id="rId2"/>
-    <hyperlink ref="D7" r:id="rId3"/>
-    <hyperlink ref="D13" r:id="rId4"/>
-    <hyperlink ref="D14" r:id="rId5"/>
-    <hyperlink ref="D20" r:id="rId6"/>
-    <hyperlink ref="D27" r:id="rId7"/>
+    <hyperlink ref="D6" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D13" r:id="rId3"/>
+    <hyperlink ref="D14" r:id="rId4"/>
+    <hyperlink ref="D20" r:id="rId5"/>
+    <hyperlink ref="D27" r:id="rId6"/>
+    <hyperlink ref="D34" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
@@ -4799,7 +4798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R324"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4891,7 +4890,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>15</v>
       </c>
@@ -4913,7 +4912,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>16</v>
       </c>
@@ -4935,7 +4934,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>17</v>
       </c>
@@ -5215,7 +5214,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>29</v>
       </c>
@@ -9485,14 +9484,14 @@
       <c r="R221" s="1"/>
     </row>
     <row r="222" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A222" s="53"/>
-      <c r="B222" s="54"/>
-      <c r="C222" s="54"/>
-      <c r="D222" s="54"/>
-      <c r="E222" s="54"/>
-      <c r="F222" s="54"/>
-      <c r="G222" s="54"/>
-      <c r="H222" s="54"/>
+      <c r="A222" s="52"/>
+      <c r="B222" s="53"/>
+      <c r="C222" s="53"/>
+      <c r="D222" s="53"/>
+      <c r="E222" s="53"/>
+      <c r="F222" s="53"/>
+      <c r="G222" s="53"/>
+      <c r="H222" s="53"/>
       <c r="I222" s="7"/>
       <c r="J222" s="1"/>
       <c r="K222" s="1"/>
@@ -9505,16 +9504,16 @@
       <c r="R222" s="1"/>
     </row>
     <row r="223" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A223" s="55" t="s">
+      <c r="A223" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="B223" s="56"/>
-      <c r="C223" s="56"/>
-      <c r="D223" s="56"/>
-      <c r="E223" s="56"/>
-      <c r="F223" s="56"/>
-      <c r="G223" s="57"/>
-      <c r="H223" s="58"/>
+      <c r="B223" s="55"/>
+      <c r="C223" s="55"/>
+      <c r="D223" s="55"/>
+      <c r="E223" s="55"/>
+      <c r="F223" s="55"/>
+      <c r="G223" s="56"/>
+      <c r="H223" s="57"/>
       <c r="I223" s="7"/>
       <c r="J223" s="1"/>
       <c r="K223" s="1"/>
@@ -9527,16 +9526,16 @@
       <c r="R223" s="1"/>
     </row>
     <row r="224" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A224" s="59" t="s">
+      <c r="A224" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B224" s="60"/>
-      <c r="C224" s="60"/>
-      <c r="D224" s="60"/>
-      <c r="E224" s="60"/>
-      <c r="F224" s="60"/>
-      <c r="G224" s="61"/>
-      <c r="H224" s="62"/>
+      <c r="B224" s="59"/>
+      <c r="C224" s="59"/>
+      <c r="D224" s="59"/>
+      <c r="E224" s="59"/>
+      <c r="F224" s="59"/>
+      <c r="G224" s="60"/>
+      <c r="H224" s="61"/>
       <c r="I224" s="7"/>
       <c r="J224" s="1"/>
       <c r="K224" s="1"/>
@@ -9549,16 +9548,16 @@
       <c r="R224" s="1"/>
     </row>
     <row r="225" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A225" s="63" t="s">
+      <c r="A225" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="B225" s="64"/>
-      <c r="C225" s="65"/>
-      <c r="D225" s="65"/>
-      <c r="E225" s="65"/>
-      <c r="F225" s="65"/>
-      <c r="G225" s="66"/>
-      <c r="H225" s="66"/>
+      <c r="B225" s="63"/>
+      <c r="C225" s="64"/>
+      <c r="D225" s="64"/>
+      <c r="E225" s="64"/>
+      <c r="F225" s="64"/>
+      <c r="G225" s="65"/>
+      <c r="H225" s="65"/>
       <c r="I225" s="7"/>
       <c r="J225" s="1"/>
       <c r="K225" s="1"/>
@@ -9571,16 +9570,16 @@
       <c r="R225" s="1"/>
     </row>
     <row r="226" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A226" s="67" t="s">
+      <c r="A226" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="B226" s="68"/>
-      <c r="C226" s="69"/>
-      <c r="D226" s="69"/>
-      <c r="E226" s="69"/>
-      <c r="F226" s="69"/>
-      <c r="G226" s="70"/>
-      <c r="H226" s="70"/>
+      <c r="B226" s="67"/>
+      <c r="C226" s="68"/>
+      <c r="D226" s="68"/>
+      <c r="E226" s="68"/>
+      <c r="F226" s="68"/>
+      <c r="G226" s="69"/>
+      <c r="H226" s="69"/>
       <c r="I226" s="7"/>
       <c r="J226" s="1"/>
       <c r="K226" s="1"/>
@@ -9715,16 +9714,16 @@
       <c r="R232" s="1"/>
     </row>
     <row r="233" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A233" s="71" t="s">
+      <c r="A233" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="B233" s="72"/>
-      <c r="C233" s="73"/>
-      <c r="D233" s="73"/>
-      <c r="E233" s="73"/>
-      <c r="F233" s="73"/>
-      <c r="G233" s="70"/>
-      <c r="H233" s="70"/>
+      <c r="B233" s="71"/>
+      <c r="C233" s="72"/>
+      <c r="D233" s="72"/>
+      <c r="E233" s="72"/>
+      <c r="F233" s="72"/>
+      <c r="G233" s="69"/>
+      <c r="H233" s="69"/>
       <c r="I233" s="7"/>
       <c r="J233" s="1"/>
       <c r="K233" s="1"/>
@@ -9737,16 +9736,16 @@
       <c r="R233" s="1"/>
     </row>
     <row r="234" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A234" s="74" t="s">
+      <c r="A234" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="B234" s="75"/>
-      <c r="C234" s="76"/>
-      <c r="D234" s="76"/>
-      <c r="E234" s="76"/>
-      <c r="F234" s="76"/>
-      <c r="G234" s="70"/>
-      <c r="H234" s="70"/>
+      <c r="B234" s="74"/>
+      <c r="C234" s="75"/>
+      <c r="D234" s="75"/>
+      <c r="E234" s="75"/>
+      <c r="F234" s="75"/>
+      <c r="G234" s="69"/>
+      <c r="H234" s="69"/>
       <c r="I234" s="7"/>
       <c r="J234" s="1"/>
       <c r="K234" s="1"/>
@@ -9881,16 +9880,16 @@
       <c r="R240" s="1"/>
     </row>
     <row r="241" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="74" t="s">
+      <c r="A241" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="B241" s="77"/>
-      <c r="C241" s="78"/>
-      <c r="D241" s="78"/>
-      <c r="E241" s="78"/>
-      <c r="F241" s="78"/>
-      <c r="G241" s="70"/>
-      <c r="H241" s="70"/>
+      <c r="B241" s="76"/>
+      <c r="C241" s="77"/>
+      <c r="D241" s="77"/>
+      <c r="E241" s="77"/>
+      <c r="F241" s="77"/>
+      <c r="G241" s="69"/>
+      <c r="H241" s="69"/>
       <c r="I241" s="7"/>
       <c r="J241" s="1"/>
       <c r="K241" s="1"/>
@@ -10025,16 +10024,16 @@
       <c r="R247" s="1"/>
     </row>
     <row r="248" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="74" t="s">
+      <c r="A248" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="B248" s="78"/>
-      <c r="C248" s="78"/>
-      <c r="D248" s="78"/>
-      <c r="E248" s="78"/>
-      <c r="F248" s="78"/>
-      <c r="G248" s="70"/>
-      <c r="H248" s="70"/>
+      <c r="B248" s="77"/>
+      <c r="C248" s="77"/>
+      <c r="D248" s="77"/>
+      <c r="E248" s="77"/>
+      <c r="F248" s="77"/>
+      <c r="G248" s="69"/>
+      <c r="H248" s="69"/>
       <c r="I248" s="7"/>
       <c r="J248" s="1"/>
       <c r="K248" s="1"/>
@@ -10169,16 +10168,16 @@
       <c r="R254" s="1"/>
     </row>
     <row r="255" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="74" t="s">
+      <c r="A255" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="B255" s="78"/>
-      <c r="C255" s="78"/>
-      <c r="D255" s="78"/>
-      <c r="E255" s="78"/>
-      <c r="F255" s="78"/>
-      <c r="G255" s="70"/>
-      <c r="H255" s="70"/>
+      <c r="B255" s="77"/>
+      <c r="C255" s="77"/>
+      <c r="D255" s="77"/>
+      <c r="E255" s="77"/>
+      <c r="F255" s="77"/>
+      <c r="G255" s="69"/>
+      <c r="H255" s="69"/>
       <c r="I255" s="7"/>
       <c r="J255" s="1"/>
       <c r="K255" s="1"/>
@@ -10313,16 +10312,16 @@
       <c r="R261" s="1"/>
     </row>
     <row r="262" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="74" t="s">
+      <c r="A262" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="B262" s="78"/>
-      <c r="C262" s="78"/>
-      <c r="D262" s="78"/>
-      <c r="E262" s="78"/>
-      <c r="F262" s="78"/>
-      <c r="G262" s="70"/>
-      <c r="H262" s="70"/>
+      <c r="B262" s="77"/>
+      <c r="C262" s="77"/>
+      <c r="D262" s="77"/>
+      <c r="E262" s="77"/>
+      <c r="F262" s="77"/>
+      <c r="G262" s="69"/>
+      <c r="H262" s="69"/>
       <c r="I262" s="7"/>
       <c r="J262" s="1"/>
       <c r="K262" s="1"/>
@@ -10457,16 +10456,16 @@
       <c r="R268" s="1"/>
     </row>
     <row r="269" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="74" t="s">
+      <c r="A269" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="B269" s="78"/>
-      <c r="C269" s="78"/>
-      <c r="D269" s="78"/>
-      <c r="E269" s="78"/>
-      <c r="F269" s="78"/>
-      <c r="G269" s="70"/>
-      <c r="H269" s="70"/>
+      <c r="B269" s="77"/>
+      <c r="C269" s="77"/>
+      <c r="D269" s="77"/>
+      <c r="E269" s="77"/>
+      <c r="F269" s="77"/>
+      <c r="G269" s="69"/>
+      <c r="H269" s="69"/>
       <c r="I269" s="7"/>
       <c r="J269" s="1"/>
       <c r="K269" s="1"/>
@@ -10601,16 +10600,16 @@
       <c r="R275" s="1"/>
     </row>
     <row r="276" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="74" t="s">
+      <c r="A276" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="B276" s="78"/>
-      <c r="C276" s="78"/>
-      <c r="D276" s="78"/>
-      <c r="E276" s="78"/>
-      <c r="F276" s="78"/>
-      <c r="G276" s="70"/>
-      <c r="H276" s="70"/>
+      <c r="B276" s="77"/>
+      <c r="C276" s="77"/>
+      <c r="D276" s="77"/>
+      <c r="E276" s="77"/>
+      <c r="F276" s="77"/>
+      <c r="G276" s="69"/>
+      <c r="H276" s="69"/>
       <c r="I276" s="7"/>
       <c r="J276" s="1"/>
       <c r="K276" s="1"/>
@@ -10745,16 +10744,16 @@
       <c r="R282" s="1"/>
     </row>
     <row r="283" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A283" s="74" t="s">
+      <c r="A283" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="B283" s="78"/>
-      <c r="C283" s="78"/>
-      <c r="D283" s="78"/>
-      <c r="E283" s="78"/>
-      <c r="F283" s="78"/>
-      <c r="G283" s="70"/>
-      <c r="H283" s="70"/>
+      <c r="B283" s="77"/>
+      <c r="C283" s="77"/>
+      <c r="D283" s="77"/>
+      <c r="E283" s="77"/>
+      <c r="F283" s="77"/>
+      <c r="G283" s="69"/>
+      <c r="H283" s="69"/>
       <c r="I283" s="7"/>
       <c r="J283" s="1"/>
       <c r="K283" s="1"/>
@@ -10889,16 +10888,16 @@
       <c r="R289" s="1"/>
     </row>
     <row r="290" spans="1:18" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A290" s="74" t="s">
+      <c r="A290" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="B290" s="78"/>
-      <c r="C290" s="78"/>
-      <c r="D290" s="78"/>
-      <c r="E290" s="78"/>
-      <c r="F290" s="78"/>
-      <c r="G290" s="70"/>
-      <c r="H290" s="70"/>
+      <c r="B290" s="77"/>
+      <c r="C290" s="77"/>
+      <c r="D290" s="77"/>
+      <c r="E290" s="77"/>
+      <c r="F290" s="77"/>
+      <c r="G290" s="69"/>
+      <c r="H290" s="69"/>
       <c r="I290" s="7"/>
       <c r="J290" s="1"/>
       <c r="K290" s="1"/>
@@ -11033,16 +11032,16 @@
       <c r="R296" s="1"/>
     </row>
     <row r="297" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A297" s="74" t="s">
+      <c r="A297" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="B297" s="78"/>
-      <c r="C297" s="78"/>
-      <c r="D297" s="78"/>
-      <c r="E297" s="78"/>
-      <c r="F297" s="78"/>
-      <c r="G297" s="70"/>
-      <c r="H297" s="70"/>
+      <c r="B297" s="77"/>
+      <c r="C297" s="77"/>
+      <c r="D297" s="77"/>
+      <c r="E297" s="77"/>
+      <c r="F297" s="77"/>
+      <c r="G297" s="69"/>
+      <c r="H297" s="69"/>
       <c r="I297" s="7"/>
       <c r="J297" s="1"/>
       <c r="K297" s="1"/>
@@ -11177,16 +11176,16 @@
       <c r="R303" s="1"/>
     </row>
     <row r="304" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="74" t="s">
+      <c r="A304" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B304" s="78"/>
-      <c r="C304" s="78"/>
-      <c r="D304" s="78"/>
-      <c r="E304" s="78"/>
-      <c r="F304" s="78"/>
-      <c r="G304" s="70"/>
-      <c r="H304" s="70"/>
+      <c r="B304" s="77"/>
+      <c r="C304" s="77"/>
+      <c r="D304" s="77"/>
+      <c r="E304" s="77"/>
+      <c r="F304" s="77"/>
+      <c r="G304" s="69"/>
+      <c r="H304" s="69"/>
       <c r="I304" s="7"/>
       <c r="J304" s="1"/>
       <c r="K304" s="1"/>
@@ -11321,16 +11320,16 @@
       <c r="R310" s="1"/>
     </row>
     <row r="311" spans="1:18" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A311" s="74" t="s">
+      <c r="A311" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="B311" s="78"/>
-      <c r="C311" s="78"/>
-      <c r="D311" s="78"/>
-      <c r="E311" s="78"/>
-      <c r="F311" s="78"/>
-      <c r="G311" s="70"/>
-      <c r="H311" s="70"/>
+      <c r="B311" s="77"/>
+      <c r="C311" s="77"/>
+      <c r="D311" s="77"/>
+      <c r="E311" s="77"/>
+      <c r="F311" s="77"/>
+      <c r="G311" s="69"/>
+      <c r="H311" s="69"/>
       <c r="I311" s="7"/>
       <c r="J311" s="1"/>
       <c r="K311" s="1"/>
@@ -11465,16 +11464,16 @@
       <c r="R317" s="1"/>
     </row>
     <row r="318" spans="1:18" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A318" s="74" t="s">
+      <c r="A318" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="B318" s="78"/>
-      <c r="C318" s="78"/>
-      <c r="D318" s="78"/>
-      <c r="E318" s="78"/>
-      <c r="F318" s="78"/>
-      <c r="G318" s="70"/>
-      <c r="H318" s="70"/>
+      <c r="B318" s="77"/>
+      <c r="C318" s="77"/>
+      <c r="D318" s="77"/>
+      <c r="E318" s="77"/>
+      <c r="F318" s="77"/>
+      <c r="G318" s="69"/>
+      <c r="H318" s="69"/>
       <c r="I318" s="7"/>
       <c r="J318" s="1"/>
       <c r="K318" s="1"/>

</xml_diff>